<commit_message>
Long time no update, worked on main thesis file and added theory and form
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ingma\OneDrive\Studie\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{0BBBBE01-06D6-4697-AB19-423295C66A96}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{9E766CB6-C50D-4AAB-8A2A-EDFBE959F135}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="1" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planning" sheetId="1" r:id="rId1"/>
+    <sheet name="Mensen in de loop" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Planning</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Plan van aanpak overleggen met begeleiders</t>
   </si>
   <si>
-    <t>Programma van eisen model en tool</t>
-  </si>
-  <si>
     <t>Manoeuvring capabilities input definieren</t>
   </si>
   <si>
@@ -97,6 +95,63 @@
   </si>
   <si>
     <t>Aantekening</t>
+  </si>
+  <si>
+    <t>Programma van eisen thesis (abstract model van onderzoek)</t>
+  </si>
+  <si>
+    <t>Toine Cleophas</t>
+  </si>
+  <si>
+    <t>Begeleider Damen</t>
+  </si>
+  <si>
+    <t>Robert Hekkenberg</t>
+  </si>
+  <si>
+    <t>Begeleider Maritiem</t>
+  </si>
+  <si>
+    <t>Mark Neerincx</t>
+  </si>
+  <si>
+    <t>Begeleider Computer science</t>
+  </si>
+  <si>
+    <t>Piet Faasse</t>
+  </si>
+  <si>
+    <t>Director Electrical &amp; Automation</t>
+  </si>
+  <si>
+    <t>Martijn de Munnik</t>
+  </si>
+  <si>
+    <t>Engineer Service, Maintenance Analysis &amp; Technical advice. Veel verstand van programeren</t>
+  </si>
+  <si>
+    <t>Hans van den Broek</t>
+  </si>
+  <si>
+    <t>STC - Lector maritieme human factors</t>
+  </si>
+  <si>
+    <t>Marcel Vermeulen</t>
+  </si>
+  <si>
+    <t>RH Marine - Sales Integrated bridge systems, helpt met ECDIS</t>
+  </si>
+  <si>
+    <t>Marin</t>
+  </si>
+  <si>
+    <t>Varende</t>
+  </si>
+  <si>
+    <t>Siebe Rooijakkers</t>
+  </si>
+  <si>
+    <t>Development, autonoom bootje TU Delft</t>
   </si>
 </sst>
 </file>
@@ -151,15 +206,15 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
@@ -187,8 +242,8 @@
     <tableColumn id="1" xr3:uid="{E87A1AF8-0878-4200-95A9-81E694C43286}" name="Planning"/>
     <tableColumn id="2" xr3:uid="{895B7E34-D3B7-402C-A34C-9F6F55706011}" name="Start" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{7B411124-92A2-4459-9D31-7CCDAB08AF45}" name="Deadline" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{12E2E626-241B-46DF-B86C-6BC4911F51AA}" name="Aantekening" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{B42D4189-46A7-4B21-8833-ED28D689B77F}" name="Werkdagen" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{12E2E626-241B-46DF-B86C-6BC4911F51AA}" name="Aantekening" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B42D4189-46A7-4B21-8833-ED28D689B77F}" name="Werkdagen" dataDxfId="0">
       <calculatedColumnFormula>NETWORKDAYS(B2,C2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -498,8 +553,8 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,10 +577,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -605,7 +660,7 @@
     </row>
     <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1">
         <v>43065</v>
@@ -620,7 +675,7 @@
     </row>
     <row r="8" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>43079</v>
@@ -635,7 +690,7 @@
     </row>
     <row r="9" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>43094</v>
@@ -650,7 +705,7 @@
     </row>
     <row r="10" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>43087</v>
@@ -665,7 +720,7 @@
     </row>
     <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>43122</v>
@@ -680,7 +735,7 @@
     </row>
     <row r="12" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>43150</v>
@@ -695,7 +750,7 @@
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>43164</v>
@@ -710,7 +765,7 @@
     </row>
     <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>43178</v>
@@ -725,7 +780,7 @@
     </row>
     <row r="15" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>43199</v>
@@ -740,7 +795,7 @@
     </row>
     <row r="16" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>43209</v>
@@ -755,7 +810,7 @@
     </row>
     <row r="17" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>43227</v>
@@ -770,7 +825,7 @@
     </row>
     <row r="18" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>43241</v>
@@ -785,7 +840,7 @@
     </row>
     <row r="19" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>43255</v>
@@ -800,7 +855,7 @@
     </row>
     <row r="20" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>43275</v>
@@ -820,4 +875,96 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A6544-6EBD-4F9F-AFAE-27519D326CAD}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wrote a bit in information chapter
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{9E766CB6-C50D-4AAB-8A2A-EDFBE959F135}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{1A6467E4-A727-4FAC-85A9-9F267A692145}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="1" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="2" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
     <sheet name="Mensen in de loop" sheetId="2" r:id="rId2"/>
+    <sheet name="Quotes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Planning</t>
   </si>
@@ -152,6 +153,36 @@
   </si>
   <si>
     <t>Development, autonoom bootje TU Delft</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>Auteur</t>
+  </si>
+  <si>
+    <t>Bron</t>
+  </si>
+  <si>
+    <t>Epictetus</t>
+  </si>
+  <si>
+    <t>Het is onmogelijk om te leren wat je denkt reeds te weten</t>
+  </si>
+  <si>
+    <t>Quote english</t>
+  </si>
+  <si>
+    <t>It is impossible for a man to learn what he thinks he already knows</t>
+  </si>
+  <si>
+    <t>Scheurkalender NewScientist 2017</t>
+  </si>
+  <si>
+    <t>Marvin Minsky</t>
+  </si>
+  <si>
+    <t>We rarely recognize how wonderful it is that a person can traverse an entire lifetime without making a single really serious mistake — like putting a fork in one's eye or using a window instead of a door.</t>
   </si>
 </sst>
 </file>
@@ -554,7 +585,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A6544-6EBD-4F9F-AFAE-27519D326CAD}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -967,4 +998,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF87472-FDAE-4C06-BCB6-BF788D854208}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added quotes to planning excel
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\iwev01\Documents\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{1A6467E4-A727-4FAC-85A9-9F267A692145}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="2" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
     <sheet name="Mensen in de loop" sheetId="2" r:id="rId2"/>
     <sheet name="Quotes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Planning</t>
   </si>
@@ -183,12 +182,33 @@
   </si>
   <si>
     <t>We rarely recognize how wonderful it is that a person can traverse an entire lifetime without making a single really serious mistake — like putting a fork in one's eye or using a window instead of a door.</t>
+  </si>
+  <si>
+    <t>Zelden staan we stil bij het wonderbaarlijke feit dat we in ons leven nooit een 'echt serieuze fout maken, zoals een vork vol eten in je oog steken in plaats van in je mond, of een huis verlaten door een raam in plaats van een deur</t>
+  </si>
+  <si>
+    <t>Life is what happens to you, while you are busy making other plans</t>
+  </si>
+  <si>
+    <t>Het leven is wat je gebeurt, terwijl je andere plannen maakt</t>
+  </si>
+  <si>
+    <t>Acda en de Munnik</t>
+  </si>
+  <si>
+    <t>Allen Saunders</t>
+  </si>
+  <si>
+    <t>But I have always found, when I was worrying, that the best thing to do was to put my mind upon something, work hard and forget what was troubling me. As a cure for worrying, work is better than whisky. Much better.</t>
+  </si>
+  <si>
+    <t>Thomas Edison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,7 +253,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -245,13 +265,13 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -267,14 +287,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C011B51-D042-4DF7-A214-69A6BC3C8278}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0">
-  <autoFilter ref="A1:E20" xr:uid="{4A7E543F-B789-4B0B-A2BF-582DE106BC5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0">
+  <autoFilter ref="A1:E20"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E87A1AF8-0878-4200-95A9-81E694C43286}" name="Planning"/>
-    <tableColumn id="2" xr3:uid="{895B7E34-D3B7-402C-A34C-9F6F55706011}" name="Start" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{7B411124-92A2-4459-9D31-7CCDAB08AF45}" name="Deadline" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{12E2E626-241B-46DF-B86C-6BC4911F51AA}" name="Aantekening" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B42D4189-46A7-4B21-8833-ED28D689B77F}" name="Werkdagen" dataDxfId="0">
+    <tableColumn id="1" name="Planning"/>
+    <tableColumn id="2" name="Start" dataDxfId="3"/>
+    <tableColumn id="3" name="Deadline" dataDxfId="2"/>
+    <tableColumn id="5" name="Aantekening" dataDxfId="1"/>
+    <tableColumn id="4" name="Werkdagen" dataDxfId="0">
       <calculatedColumnFormula>NETWORKDAYS(B2,C2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -578,13 +598,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B241F0C-225A-4236-80D5-0CA2EC09B54A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -909,7 +929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A6544-6EBD-4F9F-AFAE-27519D326CAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1001,16 +1021,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF87472-FDAE-4C06-BCB6-BF788D854208}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="141" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1046,11 +1067,36 @@
       <c r="A3" t="s">
         <v>50</v>
       </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a start for python model, added theory on collision avoidance and added research questions
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{1A6467E4-A727-4FAC-85A9-9F267A692145}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{043E9E62-4424-49FC-AFFA-A4E329583C5F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="2" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Planning</t>
   </si>
@@ -183,13 +183,19 @@
   </si>
   <si>
     <t>We rarely recognize how wonderful it is that a person can traverse an entire lifetime without making a single really serious mistake — like putting a fork in one's eye or using a window instead of a door.</t>
+  </si>
+  <si>
+    <t>Active task</t>
+  </si>
+  <si>
+    <t>Finished</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +209,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,16 +238,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -253,6 +292,11 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -267,16 +311,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C011B51-D042-4DF7-A214-69A6BC3C8278}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0">
-  <autoFilter ref="A1:E20" xr:uid="{4A7E543F-B789-4B0B-A2BF-582DE106BC5F}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C011B51-D042-4DF7-A214-69A6BC3C8278}" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0">
+  <autoFilter ref="A1:G20" xr:uid="{4A7E543F-B789-4B0B-A2BF-582DE106BC5F}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E87A1AF8-0878-4200-95A9-81E694C43286}" name="Planning"/>
-    <tableColumn id="2" xr3:uid="{895B7E34-D3B7-402C-A34C-9F6F55706011}" name="Start" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{7B411124-92A2-4459-9D31-7CCDAB08AF45}" name="Deadline" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{12E2E626-241B-46DF-B86C-6BC4911F51AA}" name="Aantekening" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B42D4189-46A7-4B21-8833-ED28D689B77F}" name="Werkdagen" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{895B7E34-D3B7-402C-A34C-9F6F55706011}" name="Start" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{7B411124-92A2-4459-9D31-7CCDAB08AF45}" name="Deadline" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{12E2E626-241B-46DF-B86C-6BC4911F51AA}" name="Aantekening" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B42D4189-46A7-4B21-8833-ED28D689B77F}" name="Werkdagen" dataDxfId="2">
       <calculatedColumnFormula>NETWORKDAYS(B2,C2)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" xr3:uid="{6E75CD73-73ED-4C68-8EAF-0F86803F98A4}" name="Active task" dataDxfId="0">
+      <calculatedColumnFormula>IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{16839F9E-1C97-4C41-99C4-B0F0AABAF5CC}" name="Finished" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -582,10 +630,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,10 +642,12 @@
     <col min="2" max="3" width="12.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,8 +663,14 @@
       <c r="E1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -628,8 +684,19 @@
         <f>NETWORKDAYS(B2,C2)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -643,8 +710,15 @@
         <f t="shared" ref="E3:E20" si="0">NETWORKDAYS(B3,C3)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -658,8 +732,15 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -673,8 +754,15 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -688,8 +776,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -703,8 +798,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -718,8 +820,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -733,8 +842,15 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -748,8 +864,15 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -763,8 +886,15 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -778,8 +908,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -793,8 +930,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -808,8 +952,15 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -823,8 +974,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -838,8 +996,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -853,8 +1018,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -868,8 +1040,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -883,8 +1062,15 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -898,8 +1084,38 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="F20" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F20">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G20">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C20">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>"AND($I$2&lt;C2;G2&lt;1)"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
@@ -1004,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF87472-FDAE-4C06-BCB6-BF788D854208}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improved python model and wrote down thesis questions
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{043E9E62-4424-49FC-AFFA-A4E329583C5F}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{2A211866-2F44-43E0-986F-DB9C69AA1638}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Planning</t>
   </si>
@@ -143,12 +143,6 @@
     <t>RH Marine - Sales Integrated bridge systems, helpt met ECDIS</t>
   </si>
   <si>
-    <t>Marin</t>
-  </si>
-  <si>
-    <t>Varende</t>
-  </si>
-  <si>
     <t>Siebe Rooijakkers</t>
   </si>
   <si>
@@ -189,6 +183,30 @@
   </si>
   <si>
     <t>Finished</t>
+  </si>
+  <si>
+    <t>Monique van der Drift</t>
+  </si>
+  <si>
+    <t>STC - Opleidings coordinator en docent</t>
+  </si>
+  <si>
+    <t>Egbert Ypma</t>
+  </si>
+  <si>
+    <t>Marin - researcher</t>
+  </si>
+  <si>
+    <t>Johan de Jong</t>
+  </si>
+  <si>
+    <t>Marin - international cooperation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R&amp;D geeft veel input </t>
+  </si>
+  <si>
+    <t>Build cases</t>
   </si>
 </sst>
 </file>
@@ -245,17 +263,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
+        <i/>
         <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
@@ -266,7 +280,11 @@
     </dxf>
     <dxf>
       <font>
-        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
@@ -311,8 +329,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C011B51-D042-4DF7-A214-69A6BC3C8278}" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0">
-  <autoFilter ref="A1:G20" xr:uid="{4A7E543F-B789-4B0B-A2BF-582DE106BC5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C011B51-D042-4DF7-A214-69A6BC3C8278}" name="Table1" displayName="Table1" ref="A1:G21" totalsRowShown="0">
+  <autoFilter ref="A1:G21" xr:uid="{4A7E543F-B789-4B0B-A2BF-582DE106BC5F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E87A1AF8-0878-4200-95A9-81E694C43286}" name="Planning"/>
     <tableColumn id="2" xr3:uid="{895B7E34-D3B7-402C-A34C-9F6F55706011}" name="Start" dataDxfId="5"/>
@@ -321,17 +339,17 @@
     <tableColumn id="4" xr3:uid="{B42D4189-46A7-4B21-8833-ED28D689B77F}" name="Werkdagen" dataDxfId="2">
       <calculatedColumnFormula>NETWORKDAYS(B2,C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6E75CD73-73ED-4C68-8EAF-0F86803F98A4}" name="Active task" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{6E75CD73-73ED-4C68-8EAF-0F86803F98A4}" name="Active task" dataDxfId="1">
       <calculatedColumnFormula>IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{16839F9E-1C97-4C41-99C4-B0F0AABAF5CC}" name="Finished" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{16839F9E-1C97-4C41-99C4-B0F0AABAF5CC}" name="Finished" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -630,10 +648,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,10 +682,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -693,7 +711,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43122</v>
+        <v>43146</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -707,7 +725,7 @@
         <v>43028</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E20" si="0">NETWORKDAYS(B3,C3)</f>
+        <f t="shared" ref="E3:E21" si="0">NETWORKDAYS(B3,C3)</f>
         <v>13</v>
       </c>
       <c r="F3" s="3">
@@ -825,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -847,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -869,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -984,17 +1002,17 @@
     </row>
     <row r="16" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1">
         <v>43209</v>
       </c>
       <c r="C16" s="1">
-        <v>43226</v>
+        <v>43220</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>NETWORKDAYS(B16,C16)</f>
+        <v>8</v>
       </c>
       <c r="F16" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
@@ -1006,17 +1024,17 @@
     </row>
     <row r="17" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>43227</v>
+        <v>43221</v>
       </c>
       <c r="C17" s="1">
-        <v>43240</v>
+        <v>43226</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F17" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
@@ -1028,13 +1046,13 @@
     </row>
     <row r="18" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>43241</v>
+        <v>43227</v>
       </c>
       <c r="C18" s="1">
-        <v>43253</v>
+        <v>43240</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
@@ -1050,17 +1068,17 @@
     </row>
     <row r="19" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>43255</v>
+        <v>43241</v>
       </c>
       <c r="C19" s="1">
-        <v>43275</v>
+        <v>43253</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
@@ -1072,28 +1090,50 @@
     </row>
     <row r="20" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43255</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43275</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F20" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>43275</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <v>43287</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F20" s="3">
-        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="F21" s="3">
+        <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F20">
+  <conditionalFormatting sqref="F2:F21">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1102,7 +1142,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1111,7 +1151,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C20">
+  <conditionalFormatting sqref="C2:C21">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>"AND($I$2&lt;C2;G2&lt;1)"</formula>
     </cfRule>
@@ -1126,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A6544-6EBD-4F9F-AFAE-27519D326CAD}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,36 +1219,58 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1232,41 +1294,41 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote first and second part on industry and this research, switched to A3 for printing
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ingma\OneDrive\Studie\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{F7F44F27-E00F-4413-A54B-C0CDE809467B}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{D713216D-9024-47F5-B945-44B657121F46}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="1" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Planning</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Loodswezen - Pilot en Board</t>
+  </si>
+  <si>
+    <t>Gijs ten Stege</t>
+  </si>
+  <si>
+    <t>Maritime Support</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43168</v>
+        <v>43172</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1172,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A6544-6EBD-4F9F-AFAE-27519D326CAD}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,6 +1291,14 @@
       </c>
       <c r="B14" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Large steps in terms of simulation testing and rewriting the report
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ingma\OneDrive\Studie\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{56EA95A2-F944-4924-ABF1-E2664D714962}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{034E1B1E-8EFF-46CF-9054-6391E629745A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="2" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Mensen in de loop" sheetId="2" r:id="rId2"/>
     <sheet name="Quotes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43203</v>
+        <v>43330</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="F16" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="F17" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="F18" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="F19" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="F20" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="F21" s="3">
         <f ca="1">IF(AND($I$2&gt;=Table1[[#This Row],[Start]],Table1[[#This Row],[Finished]]&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
@@ -1323,14 +1323,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+    <col min="3" max="3" width="93" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Concept 1 for report
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d4f24f3f093ab16/Studie/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{633E23D0-E743-4249-9CEB-A378FA6FC66C}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="00A067DACF78C1DF4BC73F0F49F8294222B4EA00" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C0390C04-815E-496D-AD6D-DC8242368CBE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8070" activeTab="2" xr2:uid="{8C9268CD-808D-4021-AFEE-719BA3615329}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t>Planning</t>
   </si>
@@ -181,9 +181,6 @@
     <t>Marvin Minsky</t>
   </si>
   <si>
-    <t>We rarely recognize how wonderful it is that a person can traverse an entire lifetime without making a single really serious mistake — like putting a fork in one's eye or using a window instead of a door.</t>
-  </si>
-  <si>
     <t>Active task</t>
   </si>
   <si>
@@ -293,6 +290,39 @@
   </si>
   <si>
     <t>Psychology today, 2009</t>
+  </si>
+  <si>
+    <t>Part I</t>
+  </si>
+  <si>
+    <t>Voorwoord</t>
+  </si>
+  <si>
+    <t>Part III</t>
+  </si>
+  <si>
+    <t>Part IV</t>
+  </si>
+  <si>
+    <t>Part II</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>We rarely recognize how wonderful it is that a person can traverse an entire lifetime without making a single really serious mistake. Like putting a fork in one's eye or using a window instead of a door.</t>
+  </si>
+  <si>
+    <t>Yuval Noah Harrari</t>
+  </si>
+  <si>
+    <t>Homo Deus</t>
+  </si>
+  <si>
+    <t>Studying history will not tell us what to choose, but at least gives us more options to choose from.</t>
+  </si>
+  <si>
+    <t>Part V</t>
   </si>
 </sst>
 </file>
@@ -769,10 +799,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -798,7 +828,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43355</v>
+        <v>43369</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,7 +1119,7 @@
     </row>
     <row r="16" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <v>43209</v>
@@ -1309,7 +1339,7 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1322,10 +1352,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
         <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,34 +1376,34 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
         <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
         <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1383,125 +1413,144 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF87472-FDAE-4C06-BCB6-BF788D854208}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
       <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
       </c>
       <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
       </c>
       <c r="C9" t="s">
         <v>81</v>
@@ -1509,16 +1558,33 @@
       <c r="D9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
         <v>83</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>84</v>
       </c>
-      <c r="D10" t="s">
-        <v>85</v>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>